<commit_message>
new flukso sensors from l'Echappee => new group
</commit_message>
<xml_diff>
--- a/sensors/FluksoTechnical.xlsx
+++ b/sensors/FluksoTechnical.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="385">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -987,36 +987,144 @@
     <t xml:space="preserve">63602be345d4d8ae3171a6bd04947d2c</t>
   </si>
   <si>
+    <t xml:space="preserve">PV_Brun</t>
+  </si>
+  <si>
     <t xml:space="preserve">28e3c147dba04c002056d5f9bd834a42</t>
   </si>
   <si>
     <t xml:space="preserve">8b4d41ebe4f3d0cd5ddd9c5cc9ee0157</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Brun-</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">89fad527d79bc1ccdfc5b556db4c13b3</t>
   </si>
   <si>
     <t xml:space="preserve">45a2eeac59d4abc4d8544d7ff11b68a9</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gris</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">19f64726ac4fb5a24e9e9fd5d3ae4faf</t>
   </si>
   <si>
     <t xml:space="preserve">2cc6fc7d84eacc63eb16222c12aebbe8</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Gris-</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">5b4b2aaa84498a6a78e047ce101ceb19</t>
   </si>
   <si>
     <t xml:space="preserve">df901ac9366a927bf2119bfa3e7a75fc</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Noir</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">5a0846b7dce5f176b06891af1ed106cf</t>
   </si>
   <si>
     <t xml:space="preserve">92c55fa626dbb3f09f5298814c5fbd1a</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Noir-</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">e4159ab40d971f6191b5d66f90ee9bac</t>
   </si>
   <si>
@@ -1093,6 +1201,27 @@
   </si>
   <si>
     <t xml:space="preserve">2d7856bbf7a791370eae5f10cd2e1002</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">PV_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Brun</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">0ef5cbd1201990d7057c1ee1f0f9d231</t>
@@ -1196,12 +1325,6 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1219,6 +1342,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1264,7 +1393,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1288,12 +1417,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1326,7 +1451,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1334,23 +1475,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1358,7 +1483,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1398,15 +1523,18 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2 3 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3915,7 +4043,7 @@
   <dimension ref="A1:L109"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A74" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C113" activeCellId="0" sqref="C113"/>
+      <selection pane="topLeft" activeCell="M105" activeCellId="0" sqref="M105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3923,7 +4051,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="17" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="9.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="17" width="9.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="17" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="7.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="36.14"/>
@@ -5821,7 +5949,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
         <v>73</v>
       </c>
@@ -5838,10 +5966,10 @@
         <v>116</v>
       </c>
       <c r="L82" s="19" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>73</v>
       </c>
@@ -5849,19 +5977,19 @@
         <v>-1</v>
       </c>
       <c r="I83" s="19" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="J83" s="19" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="K83" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L83" s="19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L83" s="26" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
         <v>73</v>
       </c>
@@ -5869,19 +5997,19 @@
         <v>1</v>
       </c>
       <c r="I84" s="19" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="J84" s="19" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="K84" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L84" s="19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L84" s="26" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
         <v>73</v>
       </c>
@@ -5889,19 +6017,19 @@
         <v>-1</v>
       </c>
       <c r="I85" s="19" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="J85" s="19" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="K85" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L85" s="19" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L85" s="26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
         <v>73</v>
       </c>
@@ -5909,19 +6037,19 @@
         <v>1</v>
       </c>
       <c r="I86" s="19" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="J86" s="19" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="K86" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L86" s="19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L86" s="26" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
         <v>73</v>
       </c>
@@ -5929,16 +6057,16 @@
         <v>-1</v>
       </c>
       <c r="I87" s="19" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="J87" s="19" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="K87" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L87" s="19" t="s">
-        <v>267</v>
+      <c r="L87" s="26" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5949,10 +6077,10 @@
         <v>1</v>
       </c>
       <c r="I88" s="19" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="J88" s="19" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="K88" s="20" t="s">
         <v>116</v>
@@ -5969,10 +6097,10 @@
         <v>-1</v>
       </c>
       <c r="I89" s="19" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="J89" s="19" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="K89" s="20" t="s">
         <v>116</v>
@@ -5989,10 +6117,10 @@
         <v>1</v>
       </c>
       <c r="I90" s="19" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="J90" s="19" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="K90" s="20" t="s">
         <v>116</v>
@@ -6009,10 +6137,10 @@
         <v>-1</v>
       </c>
       <c r="I91" s="19" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="J91" s="25" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="K91" s="20" t="s">
         <v>116</v>
@@ -6029,10 +6157,10 @@
         <v>1</v>
       </c>
       <c r="I92" s="19" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="J92" s="19" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="K92" s="20" t="s">
         <v>116</v>
@@ -6049,10 +6177,10 @@
         <v>-1</v>
       </c>
       <c r="I93" s="25" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="J93" s="19" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="K93" s="20" t="s">
         <v>116</v>
@@ -6072,10 +6200,10 @@
         <v>1</v>
       </c>
       <c r="I94" s="19" t="s">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="J94" s="19" t="s">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="K94" s="20" t="s">
         <v>116</v>
@@ -6095,10 +6223,10 @@
         <v>-1</v>
       </c>
       <c r="I95" s="19" t="s">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="J95" s="19" t="s">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="K95" s="20" t="s">
         <v>116</v>
@@ -6118,10 +6246,10 @@
         <v>1</v>
       </c>
       <c r="I96" s="19" t="s">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="J96" s="19" t="s">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="K96" s="20" t="s">
         <v>116</v>
@@ -6141,10 +6269,10 @@
         <v>-1</v>
       </c>
       <c r="I97" s="19" t="s">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="J97" s="19" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="K97" s="20" t="s">
         <v>116</v>
@@ -6164,10 +6292,10 @@
         <v>1</v>
       </c>
       <c r="I98" s="19" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="J98" s="19" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="K98" s="20" t="s">
         <v>116</v>
@@ -6187,10 +6315,10 @@
         <v>-1</v>
       </c>
       <c r="I99" s="19" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="J99" s="19" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="K99" s="20" t="s">
         <v>116</v>
@@ -6199,7 +6327,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
         <v>79</v>
       </c>
@@ -6207,19 +6335,19 @@
         <v>1</v>
       </c>
       <c r="I100" s="19" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="J100" s="19" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="K100" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="L100" s="19" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L100" s="26" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
         <v>79</v>
       </c>
@@ -6227,19 +6355,19 @@
         <v>-1</v>
       </c>
       <c r="I101" s="19" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="J101" s="19" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="K101" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L101" s="19" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L101" s="26" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
         <v>79</v>
       </c>
@@ -6247,19 +6375,19 @@
         <v>1</v>
       </c>
       <c r="I102" s="19" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="J102" s="19" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="K102" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L102" s="19" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L102" s="26" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
         <v>79</v>
       </c>
@@ -6267,19 +6395,19 @@
         <v>-1</v>
       </c>
       <c r="I103" s="19" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="J103" s="19" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="K103" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L103" s="19" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L103" s="26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
         <v>79</v>
       </c>
@@ -6287,19 +6415,19 @@
         <v>1</v>
       </c>
       <c r="I104" s="19" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="J104" s="19" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="K104" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L104" s="19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L104" s="26" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
         <v>79</v>
       </c>
@@ -6307,16 +6435,16 @@
         <v>-1</v>
       </c>
       <c r="I105" s="19" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="J105" s="19" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="K105" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="L105" s="19" t="s">
-        <v>267</v>
+      <c r="L105" s="26" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6330,16 +6458,16 @@
         <v>1</v>
       </c>
       <c r="I106" s="19" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="J106" s="19" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="K106" s="19" t="s">
         <v>116</v>
       </c>
       <c r="L106" s="19" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6353,16 +6481,16 @@
         <v>-1</v>
       </c>
       <c r="I107" s="19" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="J107" s="19" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="K107" s="20" t="s">
         <v>116</v>
       </c>
       <c r="L107" s="19" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6376,16 +6504,16 @@
         <v>1</v>
       </c>
       <c r="I108" s="19" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="J108" s="19" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="K108" s="19" t="s">
         <v>116</v>
       </c>
       <c r="L108" s="19" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6399,16 +6527,16 @@
         <v>-1</v>
       </c>
       <c r="I109" s="19" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="J109" s="19" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="K109" s="20" t="s">
         <v>116</v>
       </c>
       <c r="L109" s="19" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>